<commit_message>
Code now auto generates with the python script, but does not replace
</commit_message>
<xml_diff>
--- a/other_files/GopherCAN_message_docs.xlsx
+++ b/other_files/GopherCAN_message_docs.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\other_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBDB152-AE5D-44DD-B55B-08AAD7FA68A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BF3CCE-8A97-4A20-9295-9BC5A3C9EBE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Moduals" sheetId="1" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="3" r:id="rId2"/>
-    <sheet name="Commands" sheetId="4" r:id="rId3"/>
-    <sheet name="Errors" sheetId="6" r:id="rId4"/>
-    <sheet name="ID Example" sheetId="2" r:id="rId5"/>
-    <sheet name="Full Message Examples" sheetId="5" r:id="rId6"/>
+    <sheet name="ID Example" sheetId="2" r:id="rId1"/>
+    <sheet name="Full Message Examples" sheetId="5" r:id="rId2"/>
+    <sheet name="Moduals" sheetId="1" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="3" r:id="rId4"/>
+    <sheet name="Commands" sheetId="4" r:id="rId5"/>
+    <sheet name="Errors" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -884,518 +884,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="15.07421875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="102" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="17.07421875" customWidth="1"/>
-    <col min="2" max="2" width="25.765625" customWidth="1"/>
-    <col min="3" max="3" width="19.84375" customWidth="1"/>
-    <col min="4" max="4" width="14.69140625" customWidth="1"/>
-    <col min="5" max="5" width="23.53515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="23.69140625" customWidth="1"/>
-    <col min="4" max="4" width="17.15234375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="26.765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
@@ -1732,7 +1220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
@@ -2155,4 +1643,516 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="102" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17.07421875" customWidth="1"/>
+    <col min="2" max="2" width="25.765625" customWidth="1"/>
+    <col min="3" max="3" width="19.84375" customWidth="1"/>
+    <col min="4" max="4" width="14.69140625" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="23.69140625" customWidth="1"/>
+    <col min="4" max="4" width="17.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="26.765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified CAN commands to take 4 U8s as parameters instead of just one (UNTESTED))
</commit_message>
<xml_diff>
--- a/other_files/GopherCAN_message_docs.xlsx
+++ b/other_files/GopherCAN_message_docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\other_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\gophercan-lib\other_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BF3CCE-8A97-4A20-9295-9BC5A3C9EBE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA74A699-ABB3-407B-8A1C-758A5BB01620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID Example" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
   <si>
     <t>Module Name</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>GCAN2</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>Parameter 1</t>
+  </si>
+  <si>
+    <t>Parameter 2</t>
+  </si>
+  <si>
+    <t>Parameter 3</t>
   </si>
 </sst>
 </file>
@@ -887,17 +899,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F17:AD25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="29" width="7.61328125" customWidth="1"/>
-    <col min="31" max="31" width="11.3828125" customWidth="1"/>
+    <col min="1" max="29" width="7.6640625" customWidth="1"/>
+    <col min="31" max="31" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1064,7 +1076,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1212,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="I10" s="11"/>
@@ -1224,13 +1236,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>0</v>
       </c>
@@ -1288,7 +1300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
@@ -1344,7 +1356,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1391,7 +1403,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1414,12 +1426,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1445,7 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
         <v>71</v>
@@ -1466,7 +1478,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1486,12 +1498,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1505,13 +1517,13 @@
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="J14" t="s">
         <v>68</v>
@@ -1520,13 +1532,13 @@
         <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="O14" t="s">
         <v>59</v>
@@ -1538,7 +1550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1563,13 +1575,22 @@
       <c r="K15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="L15" t="s">
+        <v>120</v>
+      </c>
+      <c r="M15" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1583,7 +1604,7 @@
         <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
         <v>60</v>
@@ -1616,7 +1637,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1653,12 +1674,12 @@
       <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1690,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="102" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1683,7 +1704,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>109</v>
@@ -1695,7 +1716,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>112</v>
       </c>
@@ -1706,7 +1727,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>113</v>
       </c>
@@ -1717,7 +1738,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1728,7 +1749,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1739,7 +1760,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1750,7 +1771,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>110</v>
       </c>
@@ -1776,16 +1797,16 @@
       <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.07421875" customWidth="1"/>
-    <col min="2" max="2" width="25.765625" customWidth="1"/>
-    <col min="3" max="3" width="19.84375" customWidth="1"/>
-    <col min="4" max="4" width="14.69140625" customWidth="1"/>
-    <col min="5" max="5" width="23.53515625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
@@ -1799,7 +1820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="91.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1816,7 +1837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1833,7 +1854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -1847,7 +1868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1861,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>88</v>
       </c>
@@ -1875,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>89</v>
       </c>
@@ -1889,7 +1910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -1903,7 +1924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>103</v>
       </c>
@@ -1917,7 +1938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>98</v>
       </c>
@@ -1931,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>99</v>
       </c>
@@ -1945,7 +1966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>100</v>
       </c>
@@ -1959,7 +1980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>101</v>
       </c>
@@ -1973,7 +1994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>102</v>
       </c>
@@ -1987,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
   </sheetData>
@@ -2003,13 +2024,13 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.69140625" customWidth="1"/>
-    <col min="4" max="4" width="17.15234375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2041,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2032,7 +2053,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -2043,7 +2064,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>82</v>
       </c>
@@ -2054,7 +2075,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>27</v>
       </c>
@@ -2065,7 +2086,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2076,16 +2097,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.765625" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
@@ -2093,7 +2114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2104,7 +2125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>75</v>
       </c>
@@ -2112,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>79</v>
       </c>
@@ -2120,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -2128,7 +2149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -2136,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -2144,7 +2165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Updated docs to match the most recent version of the library
</commit_message>
<xml_diff>
--- a/other_files/GopherCAN_message_docs.xlsx
+++ b/other_files/GopherCAN_message_docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\gophercan-lib\other_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cal\github_files\STM32CAN\other_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA74A699-ABB3-407B-8A1C-758A5BB01620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C359BF4F-116B-4FF6-A381-3D0E238FD562}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,7 +1237,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>61</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>

</xml_diff>